<commit_message>
Comienzo api chat gpt
</commit_message>
<xml_diff>
--- a/preciosChatGPT.xlsx
+++ b/preciosChatGPT.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Coding\corunaRealEstateMarket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56371FAE-8B7A-4E6D-8756-4D500858E038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84333F2-0601-4B34-8224-A8257EDEB89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-82" yWindow="475" windowWidth="19563" windowHeight="10705" xr2:uid="{0120031D-D9B6-47DD-8D31-29C247FC6D8C}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="1" xr2:uid="{0120031D-D9B6-47DD-8D31-29C247FC6D8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>input</t>
   </si>
@@ -81,6 +82,57 @@
   </si>
   <si>
     <t>n viviendas</t>
+  </si>
+  <si>
+    <t>precio por vivienda</t>
+  </si>
+  <si>
+    <t>n tokens</t>
+  </si>
+  <si>
+    <t>prompt</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>estimacion max viviendas por call</t>
+  </si>
+  <si>
+    <t>prompt consumo %</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>input media por vivienda</t>
+  </si>
+  <si>
+    <t>output media por vivienda</t>
+  </si>
+  <si>
+    <t>total tokens</t>
+  </si>
+  <si>
+    <t>precio input</t>
+  </si>
+  <si>
+    <t>precio output</t>
+  </si>
+  <si>
+    <t>4K</t>
+  </si>
+  <si>
+    <t>16K</t>
+  </si>
+  <si>
+    <t>tokens útiles</t>
+  </si>
+  <si>
+    <t>precio tokens utiles / tokens usados</t>
+  </si>
+  <si>
+    <t>coste total</t>
   </si>
 </sst>
 </file>
@@ -96,12 +148,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,8 +180,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E2DB80-4887-42CA-BBC2-7E85464A7A43}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -443,31 +509,19 @@
     <col min="1" max="1" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="C1">
-        <f>B4*B1</f>
-        <v>168.26923076923077</v>
-      </c>
-      <c r="D1">
-        <f>B5*B1</f>
-        <v>401.7758046614872</v>
-      </c>
-      <c r="E1">
-        <f>B6*B1</f>
-        <v>354.83870967741939</v>
-      </c>
-      <c r="F1">
-        <f>B7*B1</f>
-        <v>477.55834829443444</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <f>B1*B5</f>
+        <v>493.45284489477785</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -475,23 +529,11 @@
         <v>300</v>
       </c>
       <c r="C2">
-        <f>B4*B2</f>
-        <v>50.480769230769234</v>
-      </c>
-      <c r="D2">
-        <f>B5*B2</f>
-        <v>120.53274139844616</v>
-      </c>
-      <c r="E2">
-        <f>B6*B2</f>
-        <v>106.45161290322581</v>
-      </c>
-      <c r="F2">
-        <f>B7*B2</f>
-        <v>143.26750448833033</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C2:C3" si="0">B2*B6</f>
+        <v>104.94458653026429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -499,47 +541,29 @@
         <v>200</v>
       </c>
       <c r="C3">
-        <f>B4*B3</f>
-        <v>33.653846153846153</v>
-      </c>
-      <c r="D3">
-        <f>B5*B3</f>
-        <v>80.355160932297437</v>
-      </c>
-      <c r="E3">
-        <f>B6*B3</f>
-        <v>70.967741935483872</v>
-      </c>
-      <c r="F3">
-        <f>B7*B3</f>
+        <f t="shared" si="0"/>
         <v>95.511669658886888</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <f>35/208</f>
-        <v>0.16826923076923078</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <f>362/901</f>
-        <v>0.40177580466148721</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <f>487/1283</f>
+        <v>0.37957911145752143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <f>297/837</f>
-        <v>0.35483870967741937</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <f>1231/3519</f>
+        <v>0.34981528843421428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -548,7 +572,7 @@
         <v>0.47755834829443444</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -560,7 +584,7 @@
         <f>0.06/1000</f>
         <v>5.9999999999999995E-5</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <f>0.0015/1000</f>
         <v>1.5E-6</v>
       </c>
@@ -569,7 +593,7 @@
         <v>3.0000000000000001E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -581,7 +605,7 @@
         <f>0.12/1000</f>
         <v>1.1999999999999999E-4</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <f>0.002/1000</f>
         <v>1.9999999999999999E-6</v>
       </c>
@@ -590,56 +614,59 @@
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>500</v>
+        <f>B15</f>
+        <v>10</v>
       </c>
       <c r="D15">
-        <v>500</v>
+        <f t="shared" ref="D15:E15" si="1">C15</f>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16">
         <f>B1*B5*B10</f>
-        <v>1.2053274139844614E-2</v>
+        <v>1.4803585346843335E-2</v>
       </c>
       <c r="C16">
         <f>B1*B5*C10</f>
-        <v>2.4106548279689229E-2</v>
+        <v>2.9607170693686669E-2</v>
       </c>
       <c r="D16">
         <f>B1*B5*D10</f>
-        <v>6.0266370699223084E-4</v>
+        <v>7.4017926734216684E-4</v>
       </c>
       <c r="E16">
         <f>B1*B5*E10</f>
-        <v>1.2053274139844617E-3</v>
+        <v>1.4803585346843337E-3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -648,29 +675,261 @@
       </c>
       <c r="B17">
         <f>B10*(B1*B5+B15*B2*B6) + B11*B15*B3*B7</f>
-        <v>8.9363018407698327</v>
+        <v>0.10359396310125475</v>
       </c>
       <c r="C17">
         <f>C10*(B1*B5+B15*B2*B6) + C11*B15*B3*B7</f>
-        <v>17.872603681539665</v>
+        <v>0.2071879262025095</v>
       </c>
       <c r="D17">
         <f>D10*(B1*B5+B15*B2*B6) + D11*B15*B3*B7</f>
-        <v>0.35130342237960477</v>
+        <v>4.2245814584738689E-3</v>
       </c>
       <c r="E17">
         <f>E10*(B1*B5+B15*B2*B6) + E11*B15*B3*B7</f>
-        <v>0.70260684475920954</v>
+        <v>8.4491629169477379E-3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
       <c r="B18">
         <f>B17/B15</f>
-        <v>8.9363018407698329E-3</v>
+        <v>1.0359396310125476E-2</v>
+      </c>
+      <c r="C18">
+        <f>C17/C15</f>
+        <v>2.0718792620250951E-2</v>
+      </c>
+      <c r="D18">
+        <f>D17/D15</f>
+        <v>4.2245814584738692E-4</v>
       </c>
       <c r="E18">
         <f>E17/E15</f>
-        <v>1.4052136895184191E-3</v>
+        <v>8.4491629169477383E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <f>C1+B15*C2+B15*C3</f>
+        <v>2498.0154067862895</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10A03C6-D68C-4349-9B4B-A3A23FE7DD2B}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.25" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>1223</v>
+      </c>
+      <c r="C3">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <f>100*B3/B12</f>
+        <v>81.533333333333331</v>
+      </c>
+      <c r="C4">
+        <f>100*C3/C12</f>
+        <v>7.464599609375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1669</v>
+      </c>
+      <c r="C5">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <f>B5/B2</f>
+        <v>139.08333333333334</v>
+      </c>
+      <c r="C6">
+        <f>C5/C2</f>
+        <v>139.08333333333334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>682</v>
+      </c>
+      <c r="C7">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <f>B7/B2</f>
+        <v>56.833333333333336</v>
+      </c>
+      <c r="C8">
+        <f>C7/C2</f>
+        <v>56.833333333333336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <f>B3+B5+B7</f>
+        <v>3574</v>
+      </c>
+      <c r="C9">
+        <f>C3+C5+C7</f>
+        <v>3574</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <f>B12-B3</f>
+        <v>277</v>
+      </c>
+      <c r="C11">
+        <f>C12-C3</f>
+        <v>15161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>1500</v>
+      </c>
+      <c r="C12">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1">
+        <f>(B12-B3)/(B6+B8)</f>
+        <v>1.4138664398128455</v>
+      </c>
+      <c r="C13" s="1">
+        <f>(C12-C3)/(C6+C8)</f>
+        <v>77.384942577626532</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <f>0.0015/1000</f>
+        <v>1.5E-6</v>
+      </c>
+      <c r="C15">
+        <f>0.003/1000</f>
+        <v>3.0000000000000001E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <f>0.002/1000</f>
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="C16">
+        <f>0.004/1000</f>
+        <v>3.9999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <f>(B3+B13*B6)*B15+(B13*B8)*B16</f>
+        <v>2.2901773713313485E-3</v>
+      </c>
+      <c r="C17">
+        <f>(C3+C13*C6)*C15+(C13*C8)*C16</f>
+        <v>5.3550044236495106E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <f>1000000*B17/B11</f>
+        <v>8.267788344156493</v>
+      </c>
+      <c r="C18">
+        <f>1000000*C17/C11</f>
+        <v>3.53209183012302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>